<commit_message>
review ANLT600 Test 1
</commit_message>
<xml_diff>
--- a/Fall-Semester/ANLT600/Formulas.xlsx
+++ b/Fall-Semester/ANLT600/Formulas.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae9dc2046ad84b81/Documents/SaskPolytech/SaskPolytech-AIDA-2425/Fall-Semester/ANLT600/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="261" documentId="8_{169A1F09-F5D1-0F4D-A8EE-4EC3878C25F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4199786B-0F72-DD45-96A2-154B632D2385}"/>
+  <xr:revisionPtr revIDLastSave="675" documentId="8_{169A1F09-F5D1-0F4D-A8EE-4EC3878C25F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25C96FEC-BDE3-804E-BA59-2866A63E3B79}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="500" windowWidth="27500" windowHeight="17500" activeTab="2" xr2:uid="{CDC10488-EA6D-B84A-8228-A1D2BAF6B0FA}"/>
+    <workbookView xWindow="1300" yWindow="500" windowWidth="27500" windowHeight="17500" activeTab="6" xr2:uid="{CDC10488-EA6D-B84A-8228-A1D2BAF6B0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="SimpleInterest" sheetId="6" r:id="rId1"/>
     <sheet name="PV@SimpleI" sheetId="7" r:id="rId2"/>
     <sheet name="PV@I-BearingDebt" sheetId="8" r:id="rId3"/>
     <sheet name="CompoundAmt" sheetId="1" r:id="rId4"/>
-    <sheet name="FindPresentValue" sheetId="2" r:id="rId5"/>
-    <sheet name="Review" sheetId="3" r:id="rId6"/>
-    <sheet name="Cost" sheetId="4" r:id="rId7"/>
-    <sheet name="Net Income Using TR&amp;TC" sheetId="5" r:id="rId8"/>
+    <sheet name="CompoundAmt@ChangingRate" sheetId="9" r:id="rId5"/>
+    <sheet name="PV@CompoundAmt" sheetId="2" r:id="rId6"/>
+    <sheet name="Review" sheetId="3" r:id="rId7"/>
+    <sheet name="Cost" sheetId="4" r:id="rId8"/>
+    <sheet name="Net Income Using TR&amp;TC" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="65">
   <si>
     <t>S</t>
   </si>
@@ -81,42 +82,24 @@
     <t>Sc</t>
   </si>
   <si>
-    <t>FV</t>
-  </si>
-  <si>
     <t>PV</t>
   </si>
   <si>
-    <t>P = S(1+i)^-n</t>
-  </si>
-  <si>
     <t>E4</t>
   </si>
   <si>
     <t>E6</t>
   </si>
   <si>
-    <t>i=Prt</t>
-  </si>
-  <si>
     <t>3 months</t>
   </si>
   <si>
-    <t>PV=S(1+rt)^-1</t>
-  </si>
-  <si>
     <t>E10</t>
   </si>
   <si>
     <t>E13</t>
   </si>
   <si>
-    <t>PV=S(1+r/csa)^-n</t>
-  </si>
-  <si>
-    <t>n=csa*t</t>
-  </si>
-  <si>
     <t>UVC</t>
   </si>
   <si>
@@ -223,6 +206,39 @@
   </si>
   <si>
     <t>P20</t>
+  </si>
+  <si>
+    <t>S=P(1+i)^n</t>
+  </si>
+  <si>
+    <t>Sd</t>
+  </si>
+  <si>
+    <t>P25</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>S = P(1+i)^n</t>
+  </si>
+  <si>
+    <t>P29</t>
+  </si>
+  <si>
+    <t>P32</t>
+  </si>
+  <si>
+    <t>P33</t>
   </si>
 </sst>
 </file>
@@ -297,6 +313,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -626,17 +646,17 @@
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -650,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -692,10 +712,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>1100</v>
@@ -714,7 +734,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>3500</v>
@@ -732,7 +752,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C12">
         <f>F12/(D12*E12)</f>
@@ -751,7 +771,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C13">
         <v>95000</v>
@@ -769,7 +789,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C14">
         <v>15000</v>
@@ -788,7 +808,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>15000</v>
@@ -807,7 +827,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>8000</v>
@@ -826,7 +846,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>8000</v>
@@ -844,7 +864,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <f>F18/(D18*E18)</f>
@@ -862,7 +882,7 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <f>F19/(D19*E19)</f>
@@ -880,7 +900,7 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>20000</v>
@@ -918,15 +938,15 @@
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -940,7 +960,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -986,7 +1006,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1065,15 +1085,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E2209B0-EE1C-8544-A1EA-835DA9649317}">
   <dimension ref="A2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1087,13 +1107,13 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1211,7 +1231,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1355,19 +1375,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F7906C-947A-4440-A398-6A7705D2FFA0}">
-  <dimension ref="A2:J16"/>
+  <dimension ref="A2:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="23.6640625" customWidth="1"/>
-    <col min="9" max="10" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.6640625" customWidth="1"/>
+    <col min="10" max="11" width="23.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1375,7 +1395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1383,7 +1403,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1391,7 +1411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1399,205 +1419,593 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
         <v>0</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I9" t="s">
         <v>9</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J9" t="s">
         <v>10</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <f>B8*(1+(D8/F8))^(F8*E8)</f>
-        <v>112550.88099999999</v>
-      </c>
-      <c r="B8">
-        <v>100000</v>
-      </c>
-      <c r="D8">
-        <v>0.06</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="H8" s="1">
-        <f>FindPresentValue!B10*A9*A10</f>
-        <v>871717398963992.62</v>
-      </c>
-      <c r="I8" s="1">
-        <f>A11*A12*A13</f>
-        <v>2080744619416121</v>
-      </c>
-      <c r="J8" s="1">
-        <f>A14*A15*A16</f>
-        <v>1836251861014786.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <f t="shared" ref="A9:A16" si="0">B9*(1+(D9/F9))^(F9*E9)</f>
-        <v>134488.88242462976</v>
-      </c>
-      <c r="B9">
-        <v>100000</v>
-      </c>
-      <c r="D9">
-        <v>0.1</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
-        <f t="shared" si="0"/>
-        <v>134735.10504143508</v>
-      </c>
-      <c r="B10">
-        <v>100000</v>
+      <c r="L9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>6000</v>
       </c>
       <c r="D10">
         <v>0.15</v>
       </c>
       <c r="E10">
+        <f>D10/1</f>
+        <v>0.15</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <f>F10*1</f>
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <f>C10*(1+E10)^G10</f>
+        <v>18354.137175234362</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>6000</v>
+      </c>
+      <c r="D11">
+        <v>0.15</v>
+      </c>
+      <c r="E11">
+        <f>D11/2</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+      <c r="G11">
+        <f>F11*2</f>
+        <v>16</v>
+      </c>
+      <c r="H11">
+        <f>C11*(1+E11)^G11</f>
+        <v>19084.758925621216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>6000</v>
+      </c>
+      <c r="D12">
+        <v>0.15</v>
+      </c>
+      <c r="E12">
+        <f>D12/4</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <f>F12*4</f>
+        <v>32</v>
+      </c>
+      <c r="H12">
+        <f>C12*(1+E12)^G12</f>
+        <v>19488.150401704977</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>6000</v>
+      </c>
+      <c r="D13">
+        <v>0.15</v>
+      </c>
+      <c r="E13">
+        <f>D13/12</f>
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13">
+        <f>F13*12</f>
+        <v>96</v>
+      </c>
+      <c r="H13">
+        <f>C13*(1+E13)^G13</f>
+        <v>19773.079455010957</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <f>H15/(1+E15)^G15</f>
+        <v>6408.1647167554256</v>
+      </c>
+      <c r="D15">
+        <v>0.09</v>
+      </c>
+      <c r="E15">
+        <f>D15/4</f>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <f>5*4</f>
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="F10">
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+      <c r="K17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C18">
+        <v>5000</v>
+      </c>
+      <c r="D18">
+        <v>0.08</v>
+      </c>
+      <c r="E18">
+        <f>D18/12</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="F18">
+        <v>1.5</v>
+      </c>
+      <c r="G18">
+        <f>F18*12</f>
+        <v>18</v>
+      </c>
+      <c r="H18">
+        <f>C18*(1+E18)^G18</f>
+        <v>5635.23968350205</v>
+      </c>
+      <c r="I18">
+        <f>E18</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="L18">
+        <f>G18</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>1.2</v>
+      </c>
+      <c r="C19">
+        <v>25000</v>
+      </c>
+      <c r="D19">
+        <v>0.875</v>
+      </c>
+      <c r="E19">
+        <f>D19/4</f>
+        <v>0.21875</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <f>F19*4</f>
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:H21" si="0">C19*(1+E19)^G19</f>
+        <v>121690.60165617793</v>
+      </c>
+      <c r="I19">
+        <f>E19</f>
+        <v>0.21875</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <f>G19</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>1.3</v>
+      </c>
+      <c r="C20">
+        <v>52000</v>
+      </c>
+      <c r="D20">
+        <v>0.09</v>
+      </c>
+      <c r="E20">
+        <f>D20/2</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F20">
+        <v>2.25</v>
+      </c>
+      <c r="G20">
+        <f>F20*2</f>
+        <v>4.5</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="0"/>
+        <v>63390.861010717825</v>
+      </c>
+      <c r="I20">
+        <f>E20</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <f>G20</f>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>1.4</v>
+      </c>
+      <c r="C21">
+        <v>4000</v>
+      </c>
+      <c r="D21">
+        <v>0.11</v>
+      </c>
+      <c r="E21">
+        <f>D21/1</f>
+        <v>0.11</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21">
+        <f>F21*1</f>
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>6072.281640000002</v>
+      </c>
+      <c r="I21">
+        <f>E21</f>
+        <v>0.11</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f>G21</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <f>H22/(1+E22)^G22</f>
+        <v>3720.4695744836258</v>
+      </c>
+      <c r="D22">
+        <v>0.06</v>
+      </c>
+      <c r="E22">
+        <f>D22/2</f>
+        <v>0.03</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <f>F22*2</f>
+        <v>10</v>
+      </c>
+      <c r="H22">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>2000</v>
+      </c>
+      <c r="D23">
+        <v>0.08</v>
+      </c>
+      <c r="E23">
+        <f>D23/1</f>
+        <v>0.08</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <f>F23*1</f>
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <f>C23*(1+E23)^G23</f>
+        <v>4317.8499945455751</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <f>H24/(1+E24)^G24</f>
+        <v>5402.6888450197575</v>
+      </c>
+      <c r="D24">
+        <v>0.08</v>
+      </c>
+      <c r="E24">
+        <f>D24/1</f>
+        <v>0.08</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <f>F24*1</f>
+        <v>8</v>
+      </c>
+      <c r="H24">
+        <v>10000</v>
+      </c>
+      <c r="I24">
+        <f>C24-H23</f>
+        <v>1084.8388504741824</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>100000</v>
+      </c>
+      <c r="E27">
+        <v>0.06</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27" s="2">
+        <f>C27*(1+(E27/G27))^(G27*F27)</f>
+        <v>112550.88099999999</v>
+      </c>
+      <c r="I27" s="1" t="e">
+        <f>'PV@CompoundAmt'!#REF!*H28*H29</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J27" s="1">
+        <f>H30*H31*H32</f>
+        <v>2080744619416121</v>
+      </c>
+      <c r="K27" s="1">
+        <f>H33*H34*H35</f>
+        <v>1836251861014786.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>100000</v>
+      </c>
+      <c r="E28">
+        <v>0.1</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28" s="2">
+        <f>C28*(1+(E28/G28))^(G28*F28)</f>
+        <v>134488.88242462976</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>100000</v>
+      </c>
+      <c r="E29">
+        <v>0.15</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>12</v>
+      </c>
+      <c r="H29" s="2">
+        <f>C29*(1+(E29/G29))^(G29*F29)</f>
+        <v>134735.10504143508</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>100000</v>
+      </c>
+      <c r="E30">
+        <v>0.08</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30" s="2">
+        <f>C30*(1+(E30/G30))^(G30*F30)</f>
         <v>126531.90184960004</v>
       </c>
-      <c r="B11">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C31">
         <v>100000</v>
       </c>
-      <c r="D11">
+      <c r="E31">
+        <v>0.12</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>12</v>
+      </c>
+      <c r="H31" s="2">
+        <f>C31*(1+(E31/G31))^(G31*F31)</f>
+        <v>143076.87835915809</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>100000</v>
+      </c>
+      <c r="E32">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>12</v>
+      </c>
+      <c r="H32" s="2">
+        <f>C32*(1+(E32/G32))^(G32*F32)</f>
+        <v>114934.20292071576</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>100000</v>
+      </c>
+      <c r="E33">
+        <v>0.06</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33" s="2">
+        <f>C33*(1+(E33/G33))^(G33*F33)</f>
+        <v>112360.00000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>100000</v>
+      </c>
+      <c r="E34">
         <v>0.08</v>
       </c>
-      <c r="E11">
+      <c r="F34">
         <v>3</v>
       </c>
-      <c r="F11">
+      <c r="G34">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
-        <f t="shared" si="0"/>
-        <v>143076.87835915809</v>
-      </c>
-      <c r="B12">
+      <c r="H34" s="2">
+        <f>C34*(1+(E34/G34))^(G34*F34)</f>
+        <v>126531.90184960004</v>
+      </c>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C35">
         <v>100000</v>
       </c>
-      <c r="D12">
-        <v>0.12</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <f t="shared" si="0"/>
-        <v>114934.20292071576</v>
-      </c>
-      <c r="B13">
-        <v>100000</v>
-      </c>
-      <c r="D13">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>112360.00000000001</v>
-      </c>
-      <c r="B14">
-        <v>100000</v>
-      </c>
-      <c r="D14">
-        <v>0.06</v>
-      </c>
-      <c r="E14">
+      <c r="E35">
+        <v>0.13</v>
+      </c>
+      <c r="F35">
         <v>2</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
-        <v>126531.90184960004</v>
-      </c>
-      <c r="B15">
-        <v>100000</v>
-      </c>
-      <c r="D15">
-        <v>0.08</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
+      <c r="G35">
+        <v>4</v>
+      </c>
+      <c r="H35" s="2">
+        <f>C35*(1+(E35/G35))^(G35*F35)</f>
         <v>129157.75352963673</v>
       </c>
-      <c r="B16">
-        <v>100000</v>
-      </c>
-      <c r="D16">
-        <v>0.13</v>
-      </c>
-      <c r="E16">
-        <v>2</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="H36" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1605,168 +2013,406 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B08FA02-95C2-B344-A079-E876CD2CF0CD}">
-  <dimension ref="A2:G17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C27365-6F07-0D44-BA62-0B4EA34C65BA}">
+  <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5">
+        <v>0.03</v>
+      </c>
+      <c r="E5">
+        <f>D5/4</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="F5">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="G5">
+        <f>F5*4</f>
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <f>C5*(1+E5)^G5</f>
+        <v>11611.841423032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>11611.84</v>
+      </c>
+      <c r="D6">
+        <v>0.04</v>
+      </c>
+      <c r="E6">
+        <f>D6/2</f>
+        <v>0.02</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <f>F6*2</f>
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <f>C6*(1+E6)^G6</f>
+        <v>15940.567961799372</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <f>H6-C5</f>
+        <v>5940.5679617993719</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>20000</v>
+      </c>
+      <c r="D9">
+        <v>0.09</v>
+      </c>
+      <c r="E9">
+        <f>D9/2</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <f>F9*2</f>
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <f>C9*(1+E9)^G9</f>
+        <v>23850.372012499989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>23850.37</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <f>D10/4</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <f>F10*4</f>
+        <v>12</v>
+      </c>
+      <c r="H10">
+        <f>C10*(1+E10)^G10</f>
+        <v>32076.096067139166</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>32076.1</v>
+      </c>
+      <c r="D11">
+        <v>0.13</v>
+      </c>
+      <c r="E11">
+        <f>D11/12</f>
+        <v>1.0833333333333334E-2</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f>F11*12</f>
+        <v>48</v>
+      </c>
+      <c r="H11">
+        <f>C11*(1+E11)^G11</f>
+        <v>53802.219265099862</v>
+      </c>
+      <c r="I11">
+        <f>C9*(1+E9)^G9*(1+E10)^G10*(1+E11)^G11</f>
+        <v>53802.217208236354</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <f>H11-C9</f>
+        <v>33802.219265099862</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C14">
+        <v>11500</v>
+      </c>
+      <c r="D14">
+        <v>0.6</v>
+      </c>
+      <c r="E14">
+        <f>D14/12</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <f>F14*12</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0.8</v>
+      </c>
+      <c r="E15">
+        <f>D15/4</f>
+        <v>0.2</v>
+      </c>
+      <c r="F15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <f>F15*4</f>
+        <v>20</v>
+      </c>
+      <c r="H15">
+        <f>C14*(1+E14)^G14*(1+E15)^G15</f>
+        <v>8235324.2908234466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>5000</v>
+      </c>
+      <c r="D16">
+        <v>0.7</v>
+      </c>
+      <c r="F16">
+        <v>4.5</v>
+      </c>
+      <c r="H16">
+        <f>C16*(1+D16)^F16</f>
+        <v>54449.030408493032</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <f>H16-C16</f>
+        <v>49449.030408493032</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>100000</v>
+      </c>
+      <c r="D18">
+        <v>0.6</v>
+      </c>
+      <c r="E18">
+        <f>D18/2</f>
+        <v>0.3</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <f>F18*2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <f>D19/4</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <f>F19*4</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>0.15</v>
+      </c>
+      <c r="E20">
+        <f>D20/12</f>
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <f>F20*12</f>
+        <v>24</v>
+      </c>
+      <c r="H20" s="1">
+        <f>C18*(1+E18)^G18*(1+E19)^G19*(1+E20)^G20</f>
+        <v>517535.99325677328</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>100000</v>
+      </c>
+      <c r="D21">
+        <v>0.08</v>
+      </c>
+      <c r="E21">
+        <f>D21/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <f>F21*2</f>
         <v>6</v>
       </c>
-      <c r="B3">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>0.12</v>
+      </c>
+      <c r="E22">
+        <f>D22/12</f>
+        <v>0.01</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <f>F22*12</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E23">
+        <f>D23/12</f>
+        <v>1.1666666666666667E-2</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>12</v>
+      </c>
+      <c r="H23" s="1">
+        <f>C21*(1+E21)^G21*(1+E22)^G22*(1+E23)^G23</f>
+        <v>208074.46194161213</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>100000</v>
+      </c>
+      <c r="D24">
+        <v>0.06</v>
+      </c>
+      <c r="E24">
+        <v>0.06</v>
+      </c>
+      <c r="F24">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>0.08</v>
+      </c>
+      <c r="E25">
+        <f>D25/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25">
+        <f>F25*2</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>0.13</v>
+      </c>
+      <c r="E26">
+        <f>D26/4</f>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <f>F26*4</f>
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
-        <f>C10*(1+(E10/G10))^(G10*F10)</f>
-        <v>48107.032083192717</v>
-      </c>
-      <c r="C10">
-        <v>15000</v>
-      </c>
-      <c r="E10">
-        <v>0.12</v>
-      </c>
-      <c r="F10">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
-        <f t="shared" ref="B11:B12" si="0">C11*(1+(E11/G11))^(G11*F11)</f>
-        <v>30387.247730677995</v>
-      </c>
-      <c r="C11">
-        <v>15000</v>
-      </c>
-      <c r="E11">
-        <v>0.08</v>
-      </c>
-      <c r="F11">
-        <v>9</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
-        <f t="shared" si="0"/>
-        <v>21194.607314606492</v>
-      </c>
-      <c r="C12">
-        <v>15000</v>
-      </c>
-      <c r="E12">
-        <v>0.05</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>32150.880000000001</v>
-      </c>
-      <c r="B17">
-        <v>0.15</v>
-      </c>
-      <c r="D17">
-        <f>3+(8/12)</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <f>A17*(1+B17)^(-D17)</f>
-        <v>19259.016999667816</v>
+      <c r="H26" s="1">
+        <f>C24*(1+E24)^G24*(1+E25)^G25*(1+E26)^G26</f>
+        <v>183625.18610147864</v>
       </c>
     </row>
   </sheetData>
@@ -1775,152 +2421,189 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0E484A-AD42-7F40-B7FA-6AB99781CD2F}">
-  <dimension ref="A2:H15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B08FA02-95C2-B344-A079-E876CD2CF0CD}">
+  <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>4500</v>
+      </c>
+      <c r="D5">
+        <v>0.05</v>
+      </c>
+      <c r="E5">
+        <f>D5/2</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="G5">
+        <f>F5*2</f>
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <f>C5*(1+E5)^G5</f>
+        <v>6051.9997091083387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>6052</v>
+      </c>
+      <c r="D6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <f>C6/(1+D6)^F6</f>
+        <v>4647.3050080594658</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.9</v>
+      </c>
+      <c r="E8">
+        <f>D8/2</f>
+        <v>0.45</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f>F8*2</f>
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <f>C8/(1+E8)^G8</f>
+        <v>5.1174779741990507E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>15000</v>
+      </c>
+      <c r="D10">
+        <v>0.12</v>
+      </c>
+      <c r="E10">
+        <f>D10/2</f>
+        <v>0.06</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <f>F10*2</f>
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <f>C10*(1+E10)^G10</f>
+        <v>48107.032083192717</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0.08</v>
+      </c>
+      <c r="E11">
+        <f>D11/2</f>
+        <v>0.04</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <f>F11*2</f>
+        <v>18</v>
+      </c>
+      <c r="I11">
+        <f>H10/(1+E11)^G11</f>
+        <v>23746.983854657588</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0.05</v>
+      </c>
+      <c r="E12">
+        <f>D12/2</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F12">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12">
-        <v>15000</v>
-      </c>
-      <c r="D12">
-        <v>187.5</v>
-      </c>
-      <c r="E12">
-        <v>0.05</v>
-      </c>
-      <c r="F12">
-        <f>D12/(B12*E12)</f>
-        <v>0.25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13">
-        <v>15000</v>
-      </c>
-      <c r="E13">
-        <v>0.08</v>
-      </c>
-      <c r="F13">
-        <f>33/365</f>
-        <v>9.0410958904109592E-2</v>
-      </c>
-      <c r="H13" s="2">
-        <f>C13*(1+E13*F13)^(-1)</f>
-        <v>14892.28593188989</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f>F12*2</f>
+        <v>14</v>
+      </c>
+      <c r="I12">
+        <f>H10/(1+E12)^G12</f>
+        <v>34046.654912572434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <v>50000</v>
-      </c>
-      <c r="E14">
-        <v>0.65</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <f>C14*(1+(E14/G14))^(-(G14*F14))</f>
-        <v>2997.8591313845604</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>21</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>32150.880000000001</v>
+      </c>
+      <c r="D15">
+        <v>0.15</v>
+      </c>
+      <c r="F15">
+        <f>3+8/12</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="I15">
+        <f>C15/(1+D15)^F15</f>
+        <v>19259.01699966782</v>
       </c>
     </row>
   </sheetData>
@@ -1929,6 +2612,215 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F0E484A-AD42-7F40-B7FA-6AB99781CD2F}">
+  <dimension ref="A3:M13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>15000</v>
+      </c>
+      <c r="E5">
+        <v>187.5</v>
+      </c>
+      <c r="F5">
+        <v>0.05</v>
+      </c>
+      <c r="G5">
+        <f>E5/(C5*F5)</f>
+        <v>0.25</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>15000</v>
+      </c>
+      <c r="F6">
+        <v>0.08</v>
+      </c>
+      <c r="G6">
+        <f>33/365</f>
+        <v>9.0410958904109592E-2</v>
+      </c>
+      <c r="I6" s="2">
+        <f>D6*(1+F6*G6)^(-1)</f>
+        <v>14892.28593188989</v>
+      </c>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>50000</v>
+      </c>
+      <c r="F7">
+        <v>0.65</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f>D7*(1+(F7/H7))^(-(H7*G7))</f>
+        <v>2997.8591313845604</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>15000</v>
+      </c>
+      <c r="D11">
+        <v>0.05</v>
+      </c>
+      <c r="F11">
+        <f>I11/(C11*D11)</f>
+        <v>0.25</v>
+      </c>
+      <c r="I11">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>15000</v>
+      </c>
+      <c r="D12">
+        <v>0.08</v>
+      </c>
+      <c r="F12">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+      <c r="J12">
+        <f>C12/(1+D12*K12)</f>
+        <v>14892.28593188989</v>
+      </c>
+      <c r="K12" s="2">
+        <f>_xlfn.DAYS(L12,M12)/365</f>
+        <v>9.0410958904109592E-2</v>
+      </c>
+      <c r="L12" s="3">
+        <v>45598</v>
+      </c>
+      <c r="M12" s="3">
+        <v>45565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f>H13/(1+E13)^G13</f>
+        <v>36313.607994271159</v>
+      </c>
+      <c r="D13">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E13">
+        <f>D13/2</f>
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <f>F13*2</f>
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>50000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9271A999-3EE4-1A49-8821-5B7514BE5F5A}">
   <dimension ref="A2:H6"/>
   <sheetViews>
@@ -1940,21 +2832,21 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1978,7 +2870,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <f>214.48+186.67+166.88+13+20+27+10</f>
@@ -2002,7 +2894,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10788039-FC06-CA43-BA9A-6C028FD0C0E2}">
   <dimension ref="A2:I13"/>
   <sheetViews>
@@ -2014,42 +2906,42 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -2064,7 +2956,7 @@
         <v>10</v>
       </c>
       <c r="I8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -2085,15 +2977,15 @@
         <v>13000</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>430</v>
@@ -2114,7 +3006,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>430</v>
@@ -2132,7 +3024,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update ANLT600 Test3 & CDBM602 LO5 & COMP603 Assign2 & COMP604 Assign2
</commit_message>
<xml_diff>
--- a/Fall-Semester/ANLT600/Formulas.xlsx
+++ b/Fall-Semester/ANLT600/Formulas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ae9dc2046ad84b81/Documents/SaskPolytech/SaskPolytech-AIDA-2425/Fall-Semester/ANLT600/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1394" documentId="8_{169A1F09-F5D1-0F4D-A8EE-4EC3878C25F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87FC69D2-5138-2D45-919D-D95EA0ADCDDA}"/>
+  <xr:revisionPtr revIDLastSave="1581" documentId="8_{169A1F09-F5D1-0F4D-A8EE-4EC3878C25F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{353D1A2C-54B3-4048-9C91-095FCA257312}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="27500" windowHeight="17500" activeTab="5" xr2:uid="{CDC10488-EA6D-B84A-8228-A1D2BAF6B0FA}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="27500" windowHeight="17500" activeTab="6" xr2:uid="{CDC10488-EA6D-B84A-8228-A1D2BAF6B0FA}"/>
   </bookViews>
   <sheets>
     <sheet name="LO1" sheetId="6" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="LO3" sheetId="4" r:id="rId4"/>
     <sheet name="L04" sheetId="12" r:id="rId5"/>
     <sheet name="LO5" sheetId="13" r:id="rId6"/>
+    <sheet name="LO6" sheetId="14" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="156">
   <si>
     <t>S</t>
   </si>
@@ -416,14 +417,109 @@
   </si>
   <si>
     <t>Raw Dataset</t>
+  </si>
+  <si>
+    <t>Sum(x)</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Population Variance</t>
+  </si>
+  <si>
+    <t>m = Sum(x) / N</t>
+  </si>
+  <si>
+    <t>x-m</t>
+  </si>
+  <si>
+    <t>Population Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sqrt(variance)</t>
+  </si>
+  <si>
+    <t>Power(x-m)</t>
+  </si>
+  <si>
+    <t>Sum(Power(x-m)) / N</t>
+  </si>
+  <si>
+    <t>&amp; Standard Deviation</t>
+  </si>
+  <si>
+    <t>and Standard Deviation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deviation, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variance, </t>
+  </si>
+  <si>
+    <t>ppt2</t>
+  </si>
+  <si>
+    <t>P126</t>
+  </si>
+  <si>
+    <t>x^2</t>
+  </si>
+  <si>
+    <t>y^2</t>
+  </si>
+  <si>
+    <t>x*y</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>n*Sum(x*y)</t>
+  </si>
+  <si>
+    <t>n*Sum(x*y) - Sum(x)*Sum(y)</t>
+  </si>
+  <si>
+    <t>Sum(x)*Sum(y)</t>
+  </si>
+  <si>
+    <t>n*Sum(y^2)</t>
+  </si>
+  <si>
+    <t>n*Sum(y^2) - Sum(y)^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>r^2</t>
+  </si>
+  <si>
+    <t>m = ( n*Sum(x*y) - Sum(x)*Sum(y) ) / ( n*Sum(x^2) - Sum(x)^2 )</t>
+  </si>
+  <si>
+    <t>Sqrt( n*Sum(x^2) - Sum(x)^2 )</t>
+  </si>
+  <si>
+    <t>Sqrt( n*Sum(y^2) - Sum(y)^2 )</t>
+  </si>
+  <si>
+    <t>r = ( n*Sum(x*y) - Sum(x)*Sum(y) ) / ( Sqrt( n*Sum(x^2) - Sum(x)^2 ) * Sqrt( n*Sum(y^2) - Sum(y)^2 ) )</t>
+  </si>
+  <si>
+    <t>Sqrt( n*Sum(x^2) - Sum(x)^2 ) * Sqrt( n*Sum(y^2) - Sum(y)^2 )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -517,7 +613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -531,6 +627,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -619,8 +719,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>93720</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
@@ -639,7 +739,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Ink 4">
@@ -3181,7 +3281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9271A999-3EE4-1A49-8821-5B7514BE5F5A}">
   <dimension ref="A2:T82"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -4508,14 +4608,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F40592-273E-C140-8C39-2F0C247FBDA1}">
-  <dimension ref="A3:I20"/>
+  <dimension ref="A3:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4656,8 +4759,671 @@
         <v>124</v>
       </c>
     </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <f>B40-$B$52</f>
+        <v>-0.5</v>
+      </c>
+      <c r="D40">
+        <f>POWER(C40, 2)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="C41">
+        <f t="shared" ref="C41:C49" si="0">B41-$B$52</f>
+        <v>-3.5</v>
+      </c>
+      <c r="D41">
+        <f t="shared" ref="D41:D49" si="1">POWER(C41, 2)</f>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>-2.5</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>12.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>30.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>41</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>41</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>37</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>-4.5</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>20.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>42</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>125</v>
+      </c>
+      <c r="B50">
+        <f>SUM(B40:B49)</f>
+        <v>415</v>
+      </c>
+      <c r="D50">
+        <f>SUM(D40:D49)</f>
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>126</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52">
+        <v>41.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D53" s="13">
+        <f>D50/B51</f>
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>130</v>
+      </c>
+      <c r="C54" t="s">
+        <v>131</v>
+      </c>
+      <c r="D54" s="14">
+        <f>SQRT(D53)</f>
+        <v>2.9748949561287032</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C57" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58ACBE6A-E765-814D-8B64-3883DD7670A4}">
+  <dimension ref="B4:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H4" t="s">
+        <v>141</v>
+      </c>
+      <c r="I4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>344</v>
+      </c>
+      <c r="G5">
+        <f>POWER(E5,2)</f>
+        <v>400</v>
+      </c>
+      <c r="H5">
+        <f>POWER(F5,2)</f>
+        <v>118336</v>
+      </c>
+      <c r="I5">
+        <f>E5*F5</f>
+        <v>6880</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>226</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G14" si="0">POWER(E6,2)</f>
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H14" si="1">POWER(F6,2)</f>
+        <v>51076</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I14" si="2">E6*F6</f>
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>209</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>43681</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>2090</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>50</v>
+      </c>
+      <c r="F8">
+        <v>408</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>166464</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>65.5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>4290.25</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>15</v>
+      </c>
+      <c r="F10">
+        <v>185</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>34225</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>2775</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>9.5</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>90.25</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>350</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>122500</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>8</v>
+      </c>
+      <c r="F13">
+        <v>2.5</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>6.25</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>10</v>
+      </c>
+      <c r="F14">
+        <v>270</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>72900</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E15">
+        <f>SUM(E5:E14)</f>
+        <v>148</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:I15" si="3">SUM(F5:F14)</f>
+        <v>2069.5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>3906</v>
+      </c>
+      <c r="H15" s="13">
+        <f t="shared" si="3"/>
+        <v>613568.75</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>44396.5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <f>D5*I15</f>
+        <v>443965</v>
+      </c>
+      <c r="H18">
+        <f>D5*G15</f>
+        <v>39060</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" t="s">
+        <v>149</v>
+      </c>
+      <c r="K19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <f>E15*F15</f>
+        <v>306286</v>
+      </c>
+      <c r="H20">
+        <f>H18-POWER(E15,2)</f>
+        <v>17156</v>
+      </c>
+      <c r="K20">
+        <f>SQRT(H20)</f>
+        <v>130.98091464026353</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <f>E18-E20</f>
+        <v>137679</v>
+      </c>
+      <c r="H22">
+        <f>D5*H15</f>
+        <v>6135687.5</v>
+      </c>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>148</v>
+      </c>
+      <c r="K23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <f>H22-POWER(F15,2)</f>
+        <v>1852857.25</v>
+      </c>
+      <c r="K24">
+        <f>SQRT(H24)</f>
+        <v>1361.1969916217124</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="K26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <f>K20*K24</f>
+        <v>178290.82696818703</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D30" s="15">
+        <f>E22/K27</f>
+        <v>0.77221583600914301</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <f>POWER(D30,2)</f>
+        <v>0.59631729738329964</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>144</v>
+      </c>
+      <c r="H36" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <f>D5*I15</f>
+        <v>443965</v>
+      </c>
+      <c r="H37">
+        <f>D5*G15</f>
+        <v>39060</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>146</v>
+      </c>
+      <c r="H38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <f>E15*F15</f>
+        <v>306286</v>
+      </c>
+      <c r="H39">
+        <f>H37-POWER(E15,2)</f>
+        <v>17156</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <f>E37-E39</f>
+        <v>137679</v>
+      </c>
+    </row>
+    <row r="43" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F44" s="2">
+        <f>E41/H39</f>
+        <v>8.0251224061552815</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>